<commit_message>
add more solved problems
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="192">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/remove-duplicates-from-sorted-list/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/merge-sorted-array/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/same-tree/</t>
   </si>
   <si>
     <t xml:space="preserve">Overall strategy</t>
@@ -963,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1244,6 +1256,57 @@
         <v>6</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1458,6 +1521,9 @@
     <hyperlink ref="C14" r:id="rId13" display="https://leetcode.com/problems/sqrtx/"/>
     <hyperlink ref="C15" r:id="rId14" display="https://leetcode.com/problems/climbing-stairs/"/>
     <hyperlink ref="C16" r:id="rId15" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
+    <hyperlink ref="C17" r:id="rId16" display="https://leetcode.com/problems/merge-sorted-array/"/>
+    <hyperlink ref="C18" r:id="rId17" display="https://leetcode.com/problems/binary-tree-inorder-traversal/"/>
+    <hyperlink ref="C19" r:id="rId18" display="https://leetcode.com/problems/same-tree/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1477,111 +1543,111 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F5:F6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -1589,7 +1655,7 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1597,35 +1663,35 @@
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1662,7 +1728,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F5:F6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1676,34 +1742,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1786,7 @@
         <v>49</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F2" s="14" t="n">
         <f aca="false">INT(C2/10)</f>
@@ -1747,7 +1813,7 @@
         <v>42</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F3" s="14" t="n">
         <f aca="false">INT(C3/10)</f>
@@ -1759,7 +1825,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C4" s="16" t="n">
         <v>50</v>
@@ -1768,7 +1834,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F4" s="14" t="n">
         <f aca="false">INT(C4/10)</f>
@@ -1789,7 +1855,7 @@
         <v>48</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F5" s="14" t="n">
         <f aca="false">INT(C5/10)</f>
@@ -1801,7 +1867,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C6" s="16" t="n">
         <v>47</v>
@@ -1810,7 +1876,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F6" s="14" t="n">
         <f aca="false">INT(C6/10)</f>
@@ -1822,7 +1888,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C7" s="16" t="n">
         <v>42</v>
@@ -1831,7 +1897,7 @@
         <v>32</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F7" s="14" t="n">
         <f aca="false">INT(C7/10)</f>
@@ -1852,7 +1918,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F8" s="14" t="n">
         <f aca="false">INT(C8/10)</f>
@@ -1873,7 +1939,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F9" s="14" t="n">
         <f aca="false">INT(C9/10)</f>
@@ -1894,14 +1960,14 @@
         <v>11</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F10" s="14" t="n">
         <f aca="false">INT(C10/10)</f>
         <v>3</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,7 +1975,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C11" s="19" t="n">
         <v>23</v>
@@ -1918,7 +1984,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F11" s="14" t="n">
         <f aca="false">INT(C11/10)</f>
@@ -1930,7 +1996,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C12" s="19" t="n">
         <v>21</v>
@@ -1939,7 +2005,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F12" s="14" t="n">
         <f aca="false">INT(C12/10)</f>
@@ -1960,7 +2026,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F13" s="14" t="n">
         <f aca="false">INT(C13/10)</f>
@@ -1972,7 +2038,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C14" s="10" t="n">
         <v>18</v>
@@ -1981,7 +2047,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F14" s="14" t="n">
         <f aca="false">INT(C14/10)</f>
@@ -1993,7 +2059,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C15" s="10" t="n">
         <v>17</v>
@@ -2002,14 +2068,14 @@
         <v>18</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F15" s="14" t="n">
         <f aca="false">INT(C15/10)</f>
         <v>1</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,7 +2083,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>14</v>
@@ -2026,7 +2092,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F16" s="14" t="n">
         <f aca="false">INT(C16/10)</f>
@@ -2038,7 +2104,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C17" s="10" t="n">
         <v>14</v>
@@ -2047,7 +2113,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F17" s="14" t="n">
         <f aca="false">INT(C17/10)</f>
@@ -2059,7 +2125,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C18" s="10" t="n">
         <v>13</v>
@@ -2068,7 +2134,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F18" s="14" t="n">
         <f aca="false">INT(C18/10)</f>
@@ -2080,7 +2146,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C19" s="10" t="n">
         <v>12</v>
@@ -2089,7 +2155,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F19" s="14" t="n">
         <f aca="false">INT(C19/10)</f>
@@ -2101,7 +2167,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C20" s="10" t="n">
         <v>9</v>
@@ -2110,7 +2176,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F20" s="14" t="n">
         <f aca="false">INT(C20/10)</f>
@@ -2122,7 +2188,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C21" s="10" t="n">
         <v>8</v>
@@ -2131,7 +2197,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F21" s="14" t="n">
         <f aca="false">INT(C21/10)</f>
@@ -2143,7 +2209,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C22" s="10" t="n">
         <v>7</v>
@@ -2152,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F22" s="14" t="n">
         <f aca="false">INT(C22/10)</f>
@@ -2164,7 +2230,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C23" s="10" t="n">
         <v>5</v>
@@ -2173,7 +2239,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F23" s="14" t="n">
         <f aca="false">INT(C23/10)</f>
@@ -2185,7 +2251,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C24" s="10" t="n">
         <v>5</v>
@@ -2194,7 +2260,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F24" s="14" t="n">
         <f aca="false">INT(C24/10)</f>
@@ -2245,7 +2311,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F5:F6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2263,25 +2329,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,74 +2355,74 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="23" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="23" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="23" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="23" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="23" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>6</v>
@@ -2364,11 +2430,11 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="23" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>6</v>
@@ -2376,11 +2442,11 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="23" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>6</v>
@@ -2388,11 +2454,11 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="23" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>6</v>
@@ -2400,11 +2466,11 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="23" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>6</v>
@@ -2412,11 +2478,11 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="23" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>6</v>
@@ -2424,11 +2490,11 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="23" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>6</v>
@@ -2436,11 +2502,11 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="23" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>6</v>
@@ -2448,11 +2514,11 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="23" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>6</v>
@@ -2460,11 +2526,11 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="23" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>6</v>
@@ -2472,11 +2538,11 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="23" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>6</v>
@@ -2484,223 +2550,223 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="23" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="23" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="23" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="10" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="11" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="10" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="11" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="11" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="11" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="11" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="11" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="11" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="11" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="11" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="11" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="11" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="11" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="11" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="11" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="11" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="11" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="11" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="11" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="12"/>
       <c r="C52" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
@@ -2708,7 +2774,7 @@
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="12"/>
       <c r="C53" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
@@ -2716,7 +2782,7 @@
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="12"/>
       <c r="C54" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -2726,12 +2792,12 @@
         <v>4</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="11" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,71 +2805,71 @@
         <v>14</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="11" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="11" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="11" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="11" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="11" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="24" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="11" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add time record for a problem
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="192">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -975,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1272,8 +1272,8 @@
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>7</v>
+      <c r="E17" s="3" t="n">
+        <v>12.25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,6 +1310,7 @@
         <v>7</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>